<commit_message>
ran the script and requested quote
</commit_message>
<xml_diff>
--- a/hardware/permacam/rev_a/permacam_bom.xlsx
+++ b/hardware/permacam/rev_a/permacam_bom.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nealjack/git/permamote/hardware/permacam/rev_a/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{01AE15BA-A1D0-0142-A99A-BCDA1E2E65BF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E037B3FA-6C3E-0240-B66D-73C638DFEA65}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440"/>
+    <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="permacam_bom" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="234">
   <si>
     <t>Qty</t>
   </si>
@@ -727,7 +727,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1561,11 +1561,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A50" sqref="A49:XFD50"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2603,6 +2603,9 @@
       <c r="F40" t="s">
         <v>184</v>
       </c>
+      <c r="H40" t="s">
+        <v>181</v>
+      </c>
       <c r="I40" t="s">
         <v>233</v>
       </c>

</xml_diff>

<commit_message>
Holes for 18mm holders
</commit_message>
<xml_diff>
--- a/hardware/permacam/rev_a/permacam_bom.xlsx
+++ b/hardware/permacam/rev_a/permacam_bom.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nealjack/git/permamote/hardware/permacam/rev_a/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E037B3FA-6C3E-0240-B66D-73C638DFEA65}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60EDC9E4-02D6-BD44-9887-E31A73E6DE52}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="permacam_bom" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -1562,10 +1562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I49"/>
+  <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="I39" sqref="I39"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2835,6 +2835,12 @@
         <v>232</v>
       </c>
     </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <f>SUM(A2:A49)</f>
+        <v>80</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>